<commit_message>
add driver name on laporan detail -> kenek sheet
</commit_message>
<xml_diff>
--- a/storage/app/report-template/transaksi-detail.xlsx
+++ b/storage/app/report-template/transaksi-detail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farizhermawan/other/jmp-tracking-ho-be/storage/app/report-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66EE0D8-EE45-F04D-B1E5-7813A55520DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC73F297-ABC8-4046-A54E-D486B1A98347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8520" windowWidth="33600" windowHeight="9700" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" tabRatio="990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
@@ -18,17 +18,20 @@
     <sheet name="komisi kenek" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'komisi kenek'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'komisi kenek'!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'komisi supir'!$A$1:$J$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="2">'komisi kenek'!$A$1:$I$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="2">'komisi kenek'!$A$1:$J$1</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">'komisi supir'!$A$1:$J$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Tanggal</t>
   </si>
@@ -596,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7343B576-DFBE-7B49-A0D5-03ACA3D1E897}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -716,23 +719,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DB40F4-A878-3C49-9715-F0A2AC43ADDC}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="8" width="20.83203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="7" customWidth="1"/>
+    <col min="3" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" customWidth="1"/>
+    <col min="8" max="9" width="20.83203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,21 +746,24 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>